<commit_message>
Finishing up Dispatcher; Next -> Resolve next button
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LICENTA\L_Cross_Platform\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC26ADAF-9B32-47C3-8716-02AB6907FAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D9987D-88F4-4801-92D6-FF699FE33825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>TestAsset</t>
+  </si>
+  <si>
+    <t>Li_strURL</t>
+  </si>
+  <si>
+    <t>Li_Queue</t>
+  </si>
+  <si>
+    <t>Li_strFolder</t>
   </si>
 </sst>
 </file>
@@ -547,12 +556,12 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.59765625" customWidth="1"/>
+    <col min="1" max="1" width="43.6328125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="81.36328125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -600,7 +609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="42.75">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -612,7 +621,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.5">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1631,12 +1640,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="75.36328125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1673,7 +1682,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.5">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1684,7 +1693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.5">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1798,7 +1807,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.5">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2792,15 +2801,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" customWidth="1"/>
-    <col min="2" max="2" width="30.1328125" customWidth="1"/>
-    <col min="3" max="3" width="60.265625" customWidth="1"/>
-    <col min="4" max="26" width="65.3984375" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2847,9 +2856,30 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>